<commit_message>
More package/module changes (love java!)
</commit_message>
<xml_diff>
--- a/Stats/Datasets/Medical.xlsx
+++ b/Stats/Datasets/Medical.xlsx
@@ -1,25 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ccasement\Dropbox (Fairfield University)\MATH 2217 - Statistics I\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elucid\Desktop\Classes\Repos\General\Stats\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB30EF7-D5A6-4064-9B4C-3B8D2636224B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700"/>
+    <workbookView xWindow="13380" yWindow="0" windowWidth="10710" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Medical" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="52">
   <si>
     <t>SEX</t>
   </si>
@@ -83,12 +97,105 @@
   <si>
     <t>GLUCOSE</t>
   </si>
+  <si>
+    <t>5-Number Summary</t>
+  </si>
+  <si>
+    <t>Minimum</t>
+  </si>
+  <si>
+    <t>First Quartile (Q1)</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t>Third Quartile (Q3)</t>
+  </si>
+  <si>
+    <t>Maximum</t>
+  </si>
+  <si>
+    <t>SUMMARY OUTPUT</t>
+  </si>
+  <si>
+    <t>Regression Statistics</t>
+  </si>
+  <si>
+    <t>Multiple R</t>
+  </si>
+  <si>
+    <t>R Square</t>
+  </si>
+  <si>
+    <t>Adjusted R Square</t>
+  </si>
+  <si>
+    <t>Standard Error</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>ANOVA</t>
+  </si>
+  <si>
+    <t>Regression</t>
+  </si>
+  <si>
+    <t>Residual</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Intercept</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Significance F</t>
+  </si>
+  <si>
+    <t>Coefficients</t>
+  </si>
+  <si>
+    <t>t Stat</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>Lower 95%</t>
+  </si>
+  <si>
+    <t>Upper 95%</t>
+  </si>
+  <si>
+    <t>Lower 95.0%</t>
+  </si>
+  <si>
+    <t>Upper 95.0%</t>
+  </si>
+  <si>
+    <t>X Variable 1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,6 +326,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -405,7 +520,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -520,6 +635,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -565,7 +700,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -578,6 +713,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -635,6 +778,2801 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Medical!$G$2:$G$110</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="109"/>
+                <c:pt idx="0">
+                  <c:v>26.36</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26.88</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.29</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21.93</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28.63</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>29.77</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>38.14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>29.29</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21.52</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>26.72</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>25.13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>36.119999999999997</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>25.11</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>27.38</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>24.04</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>29.82</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>28.04</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>22.11</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>28.96</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>27.01</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>30.64</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>26.77</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>31.16</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>22.12</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>28.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27.13</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>34.99</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>30.18</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>25.97</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>33.03</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>26.82</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>31.23</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>26.74</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>30.27</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>25.05</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>27.18</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>24.01</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>26.36</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>19.940000000000001</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>24.72</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>25.67</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>25.41</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>25.82</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>30.05</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>27.99</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>28.09</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>25.12</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>27.08</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>24.06</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>31.61</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>30.19</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>24.39</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>26.09</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>24.38</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>27.78</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>21.68</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>26.49</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>28.7</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>23.96</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>25.2</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>27.06</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>23.95</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>24.87</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>30.71</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>27.29</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>24.17</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>29.86</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>31.69</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>25.01</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>26.33</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>23.43</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>30.18</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>24.81</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>24.06</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>27.22</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>28.57</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>28.09</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>32.92</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>25.51</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>25.14</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>27.13</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>20.420000000000002</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>31.22</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>26.23</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>26.36</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>24.66</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>25.86</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>26.89</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>20.5</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>25.78</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>32.520000000000003</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>24.57</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>28.59</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>22.9</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>28.12</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>20.54</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>27.73</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>24.35</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>25.6</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>24.33</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>27.54</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>28.21</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>23.5</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>26.79</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>30.96</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>19.260000000000002</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>25.38</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>19.98</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8035-40F3-9563-375B4CC3B156}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1165007455"/>
+        <c:axId val="1567381183"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1165007455"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1567381183"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1567381183"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1165007455"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Medical!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>EXERCISE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.40377486874220792"/>
+                  <c:y val="0.16137196877415"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Medical!$G$2:$G$111</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="110"/>
+                <c:pt idx="0">
+                  <c:v>26.36</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26.88</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.29</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21.93</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28.63</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>29.77</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>38.14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>29.29</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21.52</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>26.72</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>25.13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>36.119999999999997</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>25.11</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>27.38</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>24.04</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>29.82</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>28.04</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>22.11</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>28.96</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>27.01</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>30.64</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>26.77</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>31.16</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>22.12</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>28.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27.13</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>34.99</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>30.18</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>25.97</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>33.03</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>26.82</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>31.23</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>26.74</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>30.27</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>25.05</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>27.18</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>24.01</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>26.36</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>19.940000000000001</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>24.72</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>25.67</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>25.41</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>25.82</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>30.05</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>27.99</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>28.09</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>25.12</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>27.08</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>24.06</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>31.61</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>30.19</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>24.39</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>26.09</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>24.38</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>27.78</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>21.68</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>26.49</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>28.7</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>23.96</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>25.2</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>27.06</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>23.95</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>24.87</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>30.71</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>27.29</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>24.17</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>29.86</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>31.69</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>25.01</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>26.33</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>23.43</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>30.18</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>24.81</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>24.06</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>27.22</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>28.57</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>28.09</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>32.92</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>25.51</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>25.14</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>27.13</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>20.420000000000002</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>31.22</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>26.23</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>26.36</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>24.66</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>25.86</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>26.89</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>20.5</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>25.78</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>32.520000000000003</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>24.57</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>28.59</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>22.9</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>28.12</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>20.54</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>27.73</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>24.35</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>25.6</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>24.33</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>27.54</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>28.21</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>23.5</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>26.79</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>30.96</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>19.260000000000002</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>25.38</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>19.98</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Medical!$M$2:$M$111</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="110"/>
+                <c:pt idx="0">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.25</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.25</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4.25</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4.25</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.25</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>3.25</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>4.75</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>3.25</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>3.25</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>3.25</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>3.25</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>4.75</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>4.25</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>3.25</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>4.25</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>4.25</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>3.25</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>3.25</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>4.75</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>3.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8257-4905-BABC-85C17F6EB391}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="114759903"/>
+        <c:axId val="617905520"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="114759903"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="617905520"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="617905520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="114759903"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>8466</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>143933</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A30EED9F-7A98-FC15-3553-22A547540EF1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>376767</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>160866</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>71967</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>110066</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5F43359-6231-8FE8-218C-0256BB70768C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -899,29 +3837,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M111"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:AA114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" topLeftCell="I46" zoomScale="79" workbookViewId="0">
+      <selection activeCell="O83" sqref="O83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.453125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.81640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.26953125" customWidth="1"/>
     <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -961,8 +3901,11 @@
       <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Z1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1002,8 +3945,14 @@
       <c r="M2" s="2">
         <v>3.75</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Z2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA2">
+        <v>19.260000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>0</v>
       </c>
@@ -1043,8 +3992,14 @@
       <c r="M3" s="2">
         <v>3.75</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Z3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA3">
+        <v>24.66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -1084,8 +4039,14 @@
       <c r="M4" s="2">
         <v>2.75</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Z4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA4">
+        <v>26.49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -1125,8 +4086,14 @@
       <c r="M5" s="2">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Z5" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA5">
+        <v>28.57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -1166,8 +4133,14 @@
       <c r="M6" s="2">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Z6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA6">
+        <v>38.14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>0</v>
       </c>
@@ -1208,7 +4181,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>1</v>
       </c>
@@ -1249,7 +4222,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>1</v>
       </c>
@@ -1290,7 +4263,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>1</v>
       </c>
@@ -1331,7 +4304,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>1</v>
       </c>
@@ -1372,7 +4345,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>1</v>
       </c>
@@ -1413,7 +4386,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>0</v>
       </c>
@@ -1454,7 +4427,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>1</v>
       </c>
@@ -1495,7 +4468,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>1</v>
       </c>
@@ -1536,7 +4509,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>1</v>
       </c>
@@ -1577,7 +4550,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>1</v>
       </c>
@@ -1618,7 +4591,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>1</v>
       </c>
@@ -1659,7 +4632,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>0</v>
       </c>
@@ -1700,7 +4673,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>1</v>
       </c>
@@ -1741,7 +4714,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>1</v>
       </c>
@@ -1782,7 +4755,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>0</v>
       </c>
@@ -1823,7 +4796,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>0</v>
       </c>
@@ -1863,8 +4836,12 @@
       <c r="M23" s="2">
         <v>3.75</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O23">
+        <f>CORREL(G:G,M:M)</f>
+        <v>-0.37461182847415936</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>0</v>
       </c>
@@ -1905,7 +4882,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>1</v>
       </c>
@@ -1946,7 +4923,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>1</v>
       </c>
@@ -1987,7 +4964,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>1</v>
       </c>
@@ -2028,7 +5005,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>1</v>
       </c>
@@ -2069,7 +5046,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>0</v>
       </c>
@@ -2110,7 +5087,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>1</v>
       </c>
@@ -2151,7 +5128,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>1</v>
       </c>
@@ -2192,7 +5169,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>1</v>
       </c>
@@ -2233,7 +5210,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>0</v>
       </c>
@@ -2274,7 +5251,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>0</v>
       </c>
@@ -2315,7 +5292,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>0</v>
       </c>
@@ -2356,7 +5333,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>0</v>
       </c>
@@ -2397,7 +5374,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>0</v>
       </c>
@@ -2438,7 +5415,7 @@
         <v>4.25</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>1</v>
       </c>
@@ -2479,7 +5456,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>1</v>
       </c>
@@ -2520,7 +5497,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>1</v>
       </c>
@@ -2561,7 +5538,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>1</v>
       </c>
@@ -2602,7 +5579,7 @@
         <v>4.25</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>1</v>
       </c>
@@ -2643,7 +5620,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>0</v>
       </c>
@@ -2684,7 +5661,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
         <v>0</v>
       </c>
@@ -2725,7 +5702,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
         <v>0</v>
       </c>
@@ -2766,7 +5743,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
         <v>0</v>
       </c>
@@ -2807,7 +5784,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
         <v>0</v>
       </c>
@@ -2848,7 +5825,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
         <v>1</v>
       </c>
@@ -2889,7 +5866,7 @@
         <v>4.25</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
         <v>1</v>
       </c>
@@ -2930,7 +5907,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
         <v>1</v>
       </c>
@@ -2971,7 +5948,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
         <v>1</v>
       </c>
@@ -3012,7 +5989,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A52" s="2">
         <v>0</v>
       </c>
@@ -3053,7 +6030,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A53" s="2">
         <v>1</v>
       </c>
@@ -3094,7 +6071,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A54" s="2">
         <v>1</v>
       </c>
@@ -3135,7 +6112,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A55" s="2">
         <v>0</v>
       </c>
@@ -3176,7 +6153,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A56" s="2">
         <v>1</v>
       </c>
@@ -3217,7 +6194,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A57" s="2">
         <v>1</v>
       </c>
@@ -3258,7 +6235,7 @@
         <v>4.75</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A58" s="2">
         <v>1</v>
       </c>
@@ -3299,7 +6276,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A59" s="2">
         <v>0</v>
       </c>
@@ -3340,7 +6317,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A60" s="2">
         <v>1</v>
       </c>
@@ -3381,7 +6358,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A61" s="2">
         <v>1</v>
       </c>
@@ -3422,7 +6399,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A62" s="2">
         <v>0</v>
       </c>
@@ -3463,7 +6440,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A63" s="2">
         <v>1</v>
       </c>
@@ -3504,7 +6481,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A64" s="2">
         <v>0</v>
       </c>
@@ -3545,7 +6522,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A65" s="2">
         <v>0</v>
       </c>
@@ -3586,7 +6563,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A66" s="2">
         <v>0</v>
       </c>
@@ -3627,7 +6604,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A67" s="2">
         <v>0</v>
       </c>
@@ -3668,7 +6645,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A68" s="2">
         <v>0</v>
       </c>
@@ -3709,7 +6686,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A69" s="2">
         <v>0</v>
       </c>
@@ -3750,7 +6727,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A70" s="2">
         <v>1</v>
       </c>
@@ -3791,7 +6768,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A71" s="2">
         <v>0</v>
       </c>
@@ -3832,7 +6809,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A72" s="2">
         <v>1</v>
       </c>
@@ -3873,7 +6850,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A73" s="2">
         <v>0</v>
       </c>
@@ -3914,7 +6891,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A74" s="2">
         <v>0</v>
       </c>
@@ -3955,7 +6932,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A75" s="2">
         <v>1</v>
       </c>
@@ -3996,7 +6973,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A76" s="2">
         <v>1</v>
       </c>
@@ -4037,7 +7014,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A77" s="2">
         <v>0</v>
       </c>
@@ -4078,7 +7055,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A78" s="2">
         <v>1</v>
       </c>
@@ -4119,7 +7096,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A79" s="2">
         <v>1</v>
       </c>
@@ -4160,7 +7137,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A80" s="2">
         <v>1</v>
       </c>
@@ -4200,8 +7177,12 @@
       <c r="M80" s="2">
         <v>2.75</v>
       </c>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O80">
+        <f>34.123-2.13297*(3.75)</f>
+        <v>26.124362499999997</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A81" s="2">
         <v>0</v>
       </c>
@@ -4241,8 +7222,12 @@
       <c r="M81" s="2">
         <v>4.75</v>
       </c>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O81">
+        <f>28.04-O80</f>
+        <v>1.9156375000000025</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A82" s="2">
         <v>1</v>
       </c>
@@ -4283,7 +7268,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A83" s="2">
         <v>1</v>
       </c>
@@ -4323,8 +7308,12 @@
       <c r="M83" s="2">
         <v>2.75</v>
       </c>
-    </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O83">
+        <f>90/110</f>
+        <v>0.81818181818181823</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A84" s="2">
         <v>0</v>
       </c>
@@ -4365,7 +7354,7 @@
         <v>4.25</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A85" s="2">
         <v>1</v>
       </c>
@@ -4406,7 +7395,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A86" s="2">
         <v>1</v>
       </c>
@@ -4447,7 +7436,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A87" s="2">
         <v>1</v>
       </c>
@@ -4488,7 +7477,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A88" s="2">
         <v>0</v>
       </c>
@@ -4529,7 +7518,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A89" s="2">
         <v>1</v>
       </c>
@@ -4570,7 +7559,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A90" s="2">
         <v>1</v>
       </c>
@@ -4611,7 +7600,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A91" s="2">
         <v>0</v>
       </c>
@@ -4652,7 +7641,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A92" s="2">
         <v>0</v>
       </c>
@@ -4693,7 +7682,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A93" s="2">
         <v>0</v>
       </c>
@@ -4734,7 +7723,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A94" s="2">
         <v>0</v>
       </c>
@@ -4775,7 +7764,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A95" s="2">
         <v>1</v>
       </c>
@@ -4816,7 +7805,7 @@
         <v>4.25</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A96" s="2">
         <v>1</v>
       </c>
@@ -4857,7 +7846,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A97" s="2">
         <v>1</v>
       </c>
@@ -4897,8 +7886,11 @@
       <c r="M97" s="2">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O97" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="98" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A98" s="2">
         <v>1</v>
       </c>
@@ -4939,7 +7931,7 @@
         <v>4.25</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A99" s="2">
         <v>0</v>
       </c>
@@ -4979,8 +7971,12 @@
       <c r="M99" s="2">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O99" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P99" s="8"/>
+    </row>
+    <row r="100" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A100" s="2">
         <v>0</v>
       </c>
@@ -5020,8 +8016,14 @@
       <c r="M100" s="2">
         <v>3.25</v>
       </c>
-    </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O100" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P100" s="5">
+        <v>0.37461182847415914</v>
+      </c>
+    </row>
+    <row r="101" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A101" s="2">
         <v>0</v>
       </c>
@@ -5061,8 +8063,14 @@
       <c r="M101" s="2">
         <v>2.75</v>
       </c>
-    </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O101" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P101" s="5">
+        <v>0.14033402203275283</v>
+      </c>
+    </row>
+    <row r="102" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A102" s="2">
         <v>0</v>
       </c>
@@ -5102,8 +8110,14 @@
       <c r="M102" s="2">
         <v>3.25</v>
       </c>
-    </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O102" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="P102" s="5">
+        <v>0.13229976055642342</v>
+      </c>
+    </row>
+    <row r="103" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A103" s="2">
         <v>1</v>
       </c>
@@ -5143,8 +8157,14 @@
       <c r="M103" s="2">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O103" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="P103" s="5">
+        <v>3.1694811117909345</v>
+      </c>
+    </row>
+    <row r="104" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A104" s="2">
         <v>1</v>
       </c>
@@ -5184,8 +8204,14 @@
       <c r="M104" s="2">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O104" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="P104" s="6">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="105" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A105" s="2">
         <v>1</v>
       </c>
@@ -5226,7 +8252,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A106" s="2">
         <v>0</v>
       </c>
@@ -5266,8 +8292,11 @@
       <c r="M106" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O106" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="107" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A107" s="2">
         <v>0</v>
       </c>
@@ -5307,8 +8336,24 @@
       <c r="M107" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O107" s="7"/>
+      <c r="P107" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q107" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="R107" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="S107" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="T107" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="108" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A108" s="2">
         <v>0</v>
       </c>
@@ -5348,8 +8393,26 @@
       <c r="M108" s="2">
         <v>4.75</v>
       </c>
-    </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O108" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P108" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q108" s="5">
+        <v>175.46614980341155</v>
+      </c>
+      <c r="R108" s="5">
+        <v>175.46614980341155</v>
+      </c>
+      <c r="S108" s="5">
+        <v>17.466947328787558</v>
+      </c>
+      <c r="T108" s="5">
+        <v>5.9921181897006766E-5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A109" s="2">
         <v>1</v>
       </c>
@@ -5389,8 +8452,22 @@
       <c r="M109" s="2">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O109" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="P109" s="5">
+        <v>107</v>
+      </c>
+      <c r="Q109" s="5">
+        <v>1074.8803254259465</v>
+      </c>
+      <c r="R109" s="5">
+        <v>10.045610517999499</v>
+      </c>
+      <c r="S109" s="5"/>
+      <c r="T109" s="5"/>
+    </row>
+    <row r="110" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A110" s="2">
         <v>0</v>
       </c>
@@ -5430,12 +8507,110 @@
       <c r="M110" s="2">
         <v>3.75</v>
       </c>
-    </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O110" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="P110" s="6">
+        <v>108</v>
+      </c>
+      <c r="Q110" s="6">
+        <v>1250.346475229358</v>
+      </c>
+      <c r="R110" s="6"/>
+      <c r="S110" s="6"/>
+      <c r="T110" s="6"/>
+    </row>
+    <row r="111" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="L111" s="1"/>
+    </row>
+    <row r="112" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="O112" s="7"/>
+      <c r="P112" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q112" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="R112" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="S112" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="T112" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="U112" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="V112" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="W112" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="113" spans="15:23" x14ac:dyDescent="0.35">
+      <c r="O113" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="P113" s="5">
+        <v>34.1229921798341</v>
+      </c>
+      <c r="Q113" s="5">
+        <v>1.8003343143396764</v>
+      </c>
+      <c r="R113" s="5">
+        <v>18.953697603852898</v>
+      </c>
+      <c r="S113" s="5">
+        <v>5.532949077549863E-36</v>
+      </c>
+      <c r="T113" s="5">
+        <v>30.554039374330451</v>
+      </c>
+      <c r="U113" s="5">
+        <v>37.691944985337706</v>
+      </c>
+      <c r="V113" s="5">
+        <v>30.554039374330451</v>
+      </c>
+      <c r="W113" s="5">
+        <v>37.691944985337706</v>
+      </c>
+    </row>
+    <row r="114" spans="15:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="O114" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="P114" s="6">
+        <v>-2.1329713657042579</v>
+      </c>
+      <c r="Q114" s="6">
+        <v>0.51035987211303369</v>
+      </c>
+      <c r="R114" s="6">
+        <v>-4.1793477157072623</v>
+      </c>
+      <c r="S114" s="6">
+        <v>5.9921181897008013E-5</v>
+      </c>
+      <c r="T114" s="6">
+        <v>-3.1447002889861273</v>
+      </c>
+      <c r="U114" s="6">
+        <v>-1.1212424424223886</v>
+      </c>
+      <c r="V114" s="6">
+        <v>-3.1447002889861273</v>
+      </c>
+      <c r="W114" s="6">
+        <v>-1.1212424424223886</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update excel datasets (for some reason):
</commit_message>
<xml_diff>
--- a/Stats/Datasets/Medical.xlsx
+++ b/Stats/Datasets/Medical.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elucid\Desktop\Classes\Repos\General\Stats\Datasets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elucid\Desktop\Classes\Stats\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB30EF7-D5A6-4064-9B4C-3B8D2636224B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A47361-2682-4B9A-B9EB-580320CA1803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13380" yWindow="0" windowWidth="10710" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43905" yWindow="930" windowWidth="29325" windowHeight="19395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Medical" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="21">
   <si>
     <t>SEX</t>
   </si>
@@ -97,105 +97,12 @@
   <si>
     <t>GLUCOSE</t>
   </si>
-  <si>
-    <t>5-Number Summary</t>
-  </si>
-  <si>
-    <t>Minimum</t>
-  </si>
-  <si>
-    <t>First Quartile (Q1)</t>
-  </si>
-  <si>
-    <t>Median</t>
-  </si>
-  <si>
-    <t>Third Quartile (Q3)</t>
-  </si>
-  <si>
-    <t>Maximum</t>
-  </si>
-  <si>
-    <t>SUMMARY OUTPUT</t>
-  </si>
-  <si>
-    <t>Regression Statistics</t>
-  </si>
-  <si>
-    <t>Multiple R</t>
-  </si>
-  <si>
-    <t>R Square</t>
-  </si>
-  <si>
-    <t>Adjusted R Square</t>
-  </si>
-  <si>
-    <t>Standard Error</t>
-  </si>
-  <si>
-    <t>Observations</t>
-  </si>
-  <si>
-    <t>ANOVA</t>
-  </si>
-  <si>
-    <t>Regression</t>
-  </si>
-  <si>
-    <t>Residual</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Intercept</t>
-  </si>
-  <si>
-    <t>df</t>
-  </si>
-  <si>
-    <t>SS</t>
-  </si>
-  <si>
-    <t>MS</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>Significance F</t>
-  </si>
-  <si>
-    <t>Coefficients</t>
-  </si>
-  <si>
-    <t>t Stat</t>
-  </si>
-  <si>
-    <t>P-value</t>
-  </si>
-  <si>
-    <t>Lower 95%</t>
-  </si>
-  <si>
-    <t>Upper 95%</t>
-  </si>
-  <si>
-    <t>Lower 95.0%</t>
-  </si>
-  <si>
-    <t>Upper 95.0%</t>
-  </si>
-  <si>
-    <t>X Variable 1</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,14 +233,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -520,7 +419,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -635,26 +534,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -700,7 +579,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -713,14 +592,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -778,2801 +649,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Medical!$G$2:$G$110</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="109"/>
-                <c:pt idx="0">
-                  <c:v>26.36</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>26.88</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>22.29</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>26.4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>21.93</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>28.63</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>29.77</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>38.14</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>29.29</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>21.52</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>26.72</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>25.13</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>36.119999999999997</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>25.11</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>27.38</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>24.04</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>29.82</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>28.04</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>22.11</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>28.96</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>27.01</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>30.64</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>26.77</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>31.16</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>22.12</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>28.5</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>27.13</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>34.99</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>30.18</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>25.97</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>33.03</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>26.82</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>31.23</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>26.74</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>30.27</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>25.05</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>27.18</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>24.01</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>26.36</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>19.940000000000001</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>24.72</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>25.67</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>25.41</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>25.82</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>30.05</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>27.99</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>28.09</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>25.12</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>27.08</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>24.06</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>31.61</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>30.19</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>24.39</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>26.09</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>24.38</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>27.78</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>21.68</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>26.49</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>28.7</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>23.96</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>25.2</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>27.06</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>23.95</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>24.87</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>30.71</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>27.29</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>24.17</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>29.86</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>31.69</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>25.01</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>26.33</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>23.43</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>30.18</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>24.81</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>24.06</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>27.22</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>28.57</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>28.09</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>32.92</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>25.51</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>25.14</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>27.13</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>20.420000000000002</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>31.22</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>26.23</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>26.36</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>24.66</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>25.86</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>26.89</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>20.5</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>25.78</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>32.520000000000003</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>24.57</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>28.59</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>22.9</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>28.12</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>20.54</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>27.73</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>24.35</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>25.6</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>24.33</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>27.54</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>28.21</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>23.5</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>26.79</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>30.96</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>19.260000000000002</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>25.38</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>19.98</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8035-40F3-9563-375B4CC3B156}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="1165007455"/>
-        <c:axId val="1567381183"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="1165007455"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1567381183"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="1567381183"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1165007455"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Medical!$M$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>EXERCISE</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.40377486874220792"/>
-                  <c:y val="0.16137196877415"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Medical!$G$2:$G$111</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="110"/>
-                <c:pt idx="0">
-                  <c:v>26.36</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>26.88</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>22.29</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>26.4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>21.93</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>28.63</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>29.77</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>38.14</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>29.29</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>21.52</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>26.72</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>25.13</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>36.119999999999997</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>25.11</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>27.38</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>24.04</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>29.82</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>28.04</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>22.11</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>28.96</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>27.01</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>30.64</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>26.77</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>31.16</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>22.12</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>28.5</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>27.13</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>34.99</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>30.18</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>25.97</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>33.03</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>26.82</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>31.23</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>26.74</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>30.27</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>25.05</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>27.18</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>24.01</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>26.36</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>19.940000000000001</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>24.72</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>25.67</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>25.41</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>25.82</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>30.05</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>27.99</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>28.09</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>25.12</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>27.08</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>24.06</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>31.61</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>30.19</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>24.39</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>26.09</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>24.38</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>27.78</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>21.68</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>26.49</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>28.7</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>23.96</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>25.2</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>27.06</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>23.95</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>24.87</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>30.71</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>27.29</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>24.17</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>29.86</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>31.69</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>25.01</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>26.33</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>23.43</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>30.18</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>24.81</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>24.06</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>27.22</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>28.57</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>28.09</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>32.92</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>25.51</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>25.14</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>27.13</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>20.420000000000002</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>31.22</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>26.23</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>26.36</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>24.66</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>25.86</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>26.89</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>20.5</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>25.78</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>32.520000000000003</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>24.57</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>28.59</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>22.9</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>28.12</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>20.54</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>27.73</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>24.35</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>25.6</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>24.33</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>27.54</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>28.21</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>23.5</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>26.79</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>30.96</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>19.260000000000002</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>25.38</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>19.98</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Medical!$M$2:$M$111</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="110"/>
-                <c:pt idx="0">
-                  <c:v>3.75</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.75</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.75</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.25</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.25</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4.5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3.75</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2.75</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3.75</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>3.75</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2.75</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>3.75</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>3.25</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>3.75</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>2.5</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>3.75</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>3.75</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1.75</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>3.75</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>3.25</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>4.25</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>4.25</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>2.75</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>4.25</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>2.25</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>3.25</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>2.25</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>3.75</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>4.75</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>3.75</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>2.5</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>2.75</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>2.75</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>3.25</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>3.75</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>3.25</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>3.25</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>3.25</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>3.75</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>2.75</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>2.75</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>4.75</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>2.75</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>4.25</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>2.5</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>3.25</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>4.25</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>3.75</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>4.25</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>3.25</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>2.75</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>3.25</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>2.5</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>4.75</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>3.75</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8257-4905-BABC-85C17F6EB391}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="114759903"/>
-        <c:axId val="617905520"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="114759903"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="617905520"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="617905520"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="114759903"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>8466</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>143933</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A30EED9F-7A98-FC15-3553-22A547540EF1}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>376767</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>160866</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>71967</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>110066</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5F43359-6231-8FE8-218C-0256BB70768C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3839,29 +915,29 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AA114"/>
+  <dimension ref="A1:M111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I46" zoomScale="79" workbookViewId="0">
-      <selection activeCell="O83" sqref="O83"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="79" workbookViewId="0">
+      <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.26953125" customWidth="1"/>
+    <col min="10" max="10" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.28515625" customWidth="1"/>
     <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3901,11 +977,8 @@
       <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="Z1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3945,14 +1018,8 @@
       <c r="M2" s="2">
         <v>3.75</v>
       </c>
-      <c r="Z2" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA2">
-        <v>19.260000000000002</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>0</v>
       </c>
@@ -3992,14 +1059,8 @@
       <c r="M3" s="2">
         <v>3.75</v>
       </c>
-      <c r="Z3" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA3">
-        <v>24.66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -4039,14 +1100,8 @@
       <c r="M4" s="2">
         <v>2.75</v>
       </c>
-      <c r="Z4" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA4">
-        <v>26.49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -4086,14 +1141,8 @@
       <c r="M5" s="2">
         <v>4.5</v>
       </c>
-      <c r="Z5" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA5">
-        <v>28.57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -4133,14 +1182,8 @@
       <c r="M6" s="2">
         <v>3.5</v>
       </c>
-      <c r="Z6" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA6">
-        <v>38.14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>0</v>
       </c>
@@ -4181,7 +1224,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>1</v>
       </c>
@@ -4222,7 +1265,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>1</v>
       </c>
@@ -4263,7 +1306,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>1</v>
       </c>
@@ -4304,7 +1347,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>1</v>
       </c>
@@ -4345,7 +1388,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>1</v>
       </c>
@@ -4386,7 +1429,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>0</v>
       </c>
@@ -4427,7 +1470,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>1</v>
       </c>
@@ -4468,7 +1511,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>1</v>
       </c>
@@ -4509,7 +1552,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>1</v>
       </c>
@@ -4550,7 +1593,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>1</v>
       </c>
@@ -4591,7 +1634,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>1</v>
       </c>
@@ -4632,7 +1675,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>0</v>
       </c>
@@ -4673,7 +1716,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>1</v>
       </c>
@@ -4714,7 +1757,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>1</v>
       </c>
@@ -4755,7 +1798,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>0</v>
       </c>
@@ -4796,7 +1839,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>0</v>
       </c>
@@ -4836,12 +1879,8 @@
       <c r="M23" s="2">
         <v>3.75</v>
       </c>
-      <c r="O23">
-        <f>CORREL(G:G,M:M)</f>
-        <v>-0.37461182847415936</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>0</v>
       </c>
@@ -4882,7 +1921,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>1</v>
       </c>
@@ -4923,7 +1962,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>1</v>
       </c>
@@ -4964,7 +2003,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>1</v>
       </c>
@@ -5005,7 +2044,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>1</v>
       </c>
@@ -5046,7 +2085,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>0</v>
       </c>
@@ -5087,7 +2126,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>1</v>
       </c>
@@ -5128,7 +2167,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>1</v>
       </c>
@@ -5169,7 +2208,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>1</v>
       </c>
@@ -5210,7 +2249,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>0</v>
       </c>
@@ -5251,7 +2290,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>0</v>
       </c>
@@ -5292,7 +2331,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>0</v>
       </c>
@@ -5333,7 +2372,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>0</v>
       </c>
@@ -5374,7 +2413,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>0</v>
       </c>
@@ -5415,7 +2454,7 @@
         <v>4.25</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>1</v>
       </c>
@@ -5456,7 +2495,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>1</v>
       </c>
@@ -5497,7 +2536,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>1</v>
       </c>
@@ -5538,7 +2577,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>1</v>
       </c>
@@ -5579,7 +2618,7 @@
         <v>4.25</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>1</v>
       </c>
@@ -5620,7 +2659,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>0</v>
       </c>
@@ -5661,7 +2700,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>0</v>
       </c>
@@ -5702,7 +2741,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>0</v>
       </c>
@@ -5743,7 +2782,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>0</v>
       </c>
@@ -5784,7 +2823,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>0</v>
       </c>
@@ -5825,7 +2864,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>1</v>
       </c>
@@ -5866,7 +2905,7 @@
         <v>4.25</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>1</v>
       </c>
@@ -5907,7 +2946,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>1</v>
       </c>
@@ -5948,7 +2987,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>1</v>
       </c>
@@ -5989,7 +3028,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>0</v>
       </c>
@@ -6030,7 +3069,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>1</v>
       </c>
@@ -6071,7 +3110,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>1</v>
       </c>
@@ -6112,7 +3151,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>0</v>
       </c>
@@ -6153,7 +3192,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>1</v>
       </c>
@@ -6194,7 +3233,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>1</v>
       </c>
@@ -6235,7 +3274,7 @@
         <v>4.75</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>1</v>
       </c>
@@ -6276,7 +3315,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>0</v>
       </c>
@@ -6317,7 +3356,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>1</v>
       </c>
@@ -6358,7 +3397,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>1</v>
       </c>
@@ -6399,7 +3438,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>0</v>
       </c>
@@ -6440,7 +3479,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>1</v>
       </c>
@@ -6481,7 +3520,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>0</v>
       </c>
@@ -6522,7 +3561,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>0</v>
       </c>
@@ -6563,7 +3602,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>0</v>
       </c>
@@ -6604,7 +3643,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>0</v>
       </c>
@@ -6645,7 +3684,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>0</v>
       </c>
@@ -6686,7 +3725,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>0</v>
       </c>
@@ -6727,7 +3766,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>1</v>
       </c>
@@ -6768,7 +3807,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>0</v>
       </c>
@@ -6809,7 +3848,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>1</v>
       </c>
@@ -6850,7 +3889,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>0</v>
       </c>
@@ -6891,7 +3930,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>0</v>
       </c>
@@ -6932,7 +3971,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>1</v>
       </c>
@@ -6973,7 +4012,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>1</v>
       </c>
@@ -7014,7 +4053,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>0</v>
       </c>
@@ -7055,7 +4094,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>1</v>
       </c>
@@ -7096,7 +4135,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>1</v>
       </c>
@@ -7137,7 +4176,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>1</v>
       </c>
@@ -7177,12 +4216,8 @@
       <c r="M80" s="2">
         <v>2.75</v>
       </c>
-      <c r="O80">
-        <f>34.123-2.13297*(3.75)</f>
-        <v>26.124362499999997</v>
-      </c>
-    </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>0</v>
       </c>
@@ -7222,12 +4257,8 @@
       <c r="M81" s="2">
         <v>4.75</v>
       </c>
-      <c r="O81">
-        <f>28.04-O80</f>
-        <v>1.9156375000000025</v>
-      </c>
-    </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>1</v>
       </c>
@@ -7268,7 +4299,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>1</v>
       </c>
@@ -7308,12 +4339,8 @@
       <c r="M83" s="2">
         <v>2.75</v>
       </c>
-      <c r="O83">
-        <f>90/110</f>
-        <v>0.81818181818181823</v>
-      </c>
-    </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>0</v>
       </c>
@@ -7354,7 +4381,7 @@
         <v>4.25</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>1</v>
       </c>
@@ -7395,7 +4422,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>1</v>
       </c>
@@ -7436,7 +4463,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>1</v>
       </c>
@@ -7477,7 +4504,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>0</v>
       </c>
@@ -7518,7 +4545,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>1</v>
       </c>
@@ -7559,7 +4586,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>1</v>
       </c>
@@ -7600,7 +4627,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>0</v>
       </c>
@@ -7641,7 +4668,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>0</v>
       </c>
@@ -7682,7 +4709,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>0</v>
       </c>
@@ -7723,7 +4750,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>0</v>
       </c>
@@ -7764,7 +4791,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>1</v>
       </c>
@@ -7805,7 +4832,7 @@
         <v>4.25</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>1</v>
       </c>
@@ -7846,7 +4873,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="97" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>1</v>
       </c>
@@ -7886,11 +4913,8 @@
       <c r="M97" s="2">
         <v>3.5</v>
       </c>
-      <c r="O97" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="98" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>1</v>
       </c>
@@ -7931,7 +4955,7 @@
         <v>4.25</v>
       </c>
     </row>
-    <row r="99" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>0</v>
       </c>
@@ -7971,12 +4995,8 @@
       <c r="M99" s="2">
         <v>3.5</v>
       </c>
-      <c r="O99" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="P99" s="8"/>
-    </row>
-    <row r="100" spans="1:23" x14ac:dyDescent="0.35">
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>0</v>
       </c>
@@ -8016,14 +5036,8 @@
       <c r="M100" s="2">
         <v>3.25</v>
       </c>
-      <c r="O100" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="P100" s="5">
-        <v>0.37461182847415914</v>
-      </c>
-    </row>
-    <row r="101" spans="1:23" x14ac:dyDescent="0.35">
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>0</v>
       </c>
@@ -8063,14 +5077,8 @@
       <c r="M101" s="2">
         <v>2.75</v>
       </c>
-      <c r="O101" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="P101" s="5">
-        <v>0.14033402203275283</v>
-      </c>
-    </row>
-    <row r="102" spans="1:23" x14ac:dyDescent="0.35">
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>0</v>
       </c>
@@ -8110,14 +5118,8 @@
       <c r="M102" s="2">
         <v>3.25</v>
       </c>
-      <c r="O102" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="P102" s="5">
-        <v>0.13229976055642342</v>
-      </c>
-    </row>
-    <row r="103" spans="1:23" x14ac:dyDescent="0.35">
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>1</v>
       </c>
@@ -8157,14 +5159,8 @@
       <c r="M103" s="2">
         <v>3.5</v>
       </c>
-      <c r="O103" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="P103" s="5">
-        <v>3.1694811117909345</v>
-      </c>
-    </row>
-    <row r="104" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>1</v>
       </c>
@@ -8204,14 +5200,8 @@
       <c r="M104" s="2">
         <v>2.5</v>
       </c>
-      <c r="O104" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="P104" s="6">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="105" spans="1:23" x14ac:dyDescent="0.35">
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>1</v>
       </c>
@@ -8252,7 +5242,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="106" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>0</v>
       </c>
@@ -8292,11 +5282,8 @@
       <c r="M106" s="2">
         <v>4</v>
       </c>
-      <c r="O106" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="107" spans="1:23" x14ac:dyDescent="0.35">
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>0</v>
       </c>
@@ -8336,24 +5323,8 @@
       <c r="M107" s="2">
         <v>4</v>
       </c>
-      <c r="O107" s="7"/>
-      <c r="P107" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q107" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="R107" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="S107" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="T107" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="108" spans="1:23" x14ac:dyDescent="0.35">
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>0</v>
       </c>
@@ -8393,26 +5364,8 @@
       <c r="M108" s="2">
         <v>4.75</v>
       </c>
-      <c r="O108" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="P108" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q108" s="5">
-        <v>175.46614980341155</v>
-      </c>
-      <c r="R108" s="5">
-        <v>175.46614980341155</v>
-      </c>
-      <c r="S108" s="5">
-        <v>17.466947328787558</v>
-      </c>
-      <c r="T108" s="5">
-        <v>5.9921181897006766E-5</v>
-      </c>
-    </row>
-    <row r="109" spans="1:23" x14ac:dyDescent="0.35">
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>1</v>
       </c>
@@ -8452,22 +5405,8 @@
       <c r="M109" s="2">
         <v>3.5</v>
       </c>
-      <c r="O109" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="P109" s="5">
-        <v>107</v>
-      </c>
-      <c r="Q109" s="5">
-        <v>1074.8803254259465</v>
-      </c>
-      <c r="R109" s="5">
-        <v>10.045610517999499</v>
-      </c>
-      <c r="S109" s="5"/>
-      <c r="T109" s="5"/>
-    </row>
-    <row r="110" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>0</v>
       </c>
@@ -8507,110 +5446,12 @@
       <c r="M110" s="2">
         <v>3.75</v>
       </c>
-      <c r="O110" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="P110" s="6">
-        <v>108</v>
-      </c>
-      <c r="Q110" s="6">
-        <v>1250.346475229358</v>
-      </c>
-      <c r="R110" s="6"/>
-      <c r="S110" s="6"/>
-      <c r="T110" s="6"/>
-    </row>
-    <row r="111" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L111" s="1"/>
-    </row>
-    <row r="112" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="O112" s="7"/>
-      <c r="P112" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q112" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="R112" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="S112" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="T112" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="U112" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="V112" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="W112" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="113" spans="15:23" x14ac:dyDescent="0.35">
-      <c r="O113" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="P113" s="5">
-        <v>34.1229921798341</v>
-      </c>
-      <c r="Q113" s="5">
-        <v>1.8003343143396764</v>
-      </c>
-      <c r="R113" s="5">
-        <v>18.953697603852898</v>
-      </c>
-      <c r="S113" s="5">
-        <v>5.532949077549863E-36</v>
-      </c>
-      <c r="T113" s="5">
-        <v>30.554039374330451</v>
-      </c>
-      <c r="U113" s="5">
-        <v>37.691944985337706</v>
-      </c>
-      <c r="V113" s="5">
-        <v>30.554039374330451</v>
-      </c>
-      <c r="W113" s="5">
-        <v>37.691944985337706</v>
-      </c>
-    </row>
-    <row r="114" spans="15:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="O114" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="P114" s="6">
-        <v>-2.1329713657042579</v>
-      </c>
-      <c r="Q114" s="6">
-        <v>0.51035987211303369</v>
-      </c>
-      <c r="R114" s="6">
-        <v>-4.1793477157072623</v>
-      </c>
-      <c r="S114" s="6">
-        <v>5.9921181897008013E-5</v>
-      </c>
-      <c r="T114" s="6">
-        <v>-3.1447002889861273</v>
-      </c>
-      <c r="U114" s="6">
-        <v>-1.1212424424223886</v>
-      </c>
-      <c r="V114" s="6">
-        <v>-3.1447002889861273</v>
-      </c>
-      <c r="W114" s="6">
-        <v>-1.1212424424223886</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>